<commit_message>
Updating product page generation
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirilllahnov/Documents/Building_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D917B1-10DF-F741-A6B4-60E418B76065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB616717-1A0E-904B-9123-D68B834F9911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-17420" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Кровля" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>ТИП</t>
   </si>
@@ -80,6 +81,12 @@
   </si>
   <si>
     <t>img/catalog/roof/4.jpeg</t>
+  </si>
+  <si>
+    <t>asaddd</t>
+  </si>
+  <si>
+    <t>ad</t>
   </si>
 </sst>
 </file>
@@ -184,7 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -495,7 +502,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -661,4 +668,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDEA5D6-51F9-124A-8930-2910D6524229}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Product card generation update
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirilllahnov/Documents/Building_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7DFD6F-92E7-B143-A39B-FE3DD678D040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCE054E-25C6-FF4B-8B8B-B3DD3A2768EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-17420" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,34 +173,6 @@
 3000х370х170
 Вес, кг
 4.6
-Страна производства
-Россия</t>
-  </si>
-  <si>
-    <t>Тип продукта
-Профнастил
-Основной материал
-Сталь
-Цветовая палитра
-Серый / серебристый
-Цветовая палитра по RAL
-Нет
-Площадь покрытия продуктом (м²)
-2.32
-Полезная площадь (м²)
-2.09
-Длина (см)
-200
-Ширина (см)
-116
-Толщина (мм)
-0.35
-Высота волны (мм)
-20
-Вес на м² (кг)
-3,1
-Вес, кг
-6.5
 Страна производства
 Россия</t>
   </si>
@@ -284,6 +256,34 @@
 Вес, кг
 5.99
 Страна производства
+Россия</t>
+  </si>
+  <si>
+    <t>Тип продукта:
+Профнастил&lt;br&gt;
+Основной материал:
+Сталь&lt;br&gt;
+Цветовая палитра:
+Серый / серебристый&lt;br&gt;
+Цветовая палитра по RAL:
+Нет&lt;br&gt;
+Площадь покрытия продуктом (м²):
+2.32&lt;br&gt;
+Полезная площадь (м²):
+2.09&lt;br&gt;
+Длина (см):
+200&lt;br&gt;
+Ширина (см):
+116&lt;br&gt;
+Толщина (мм):
+0.35&lt;br&gt;
+Высота волны (мм):
+20&lt;br&gt;
+Вес на м² (кг):
+3,1&lt;br&gt;
+Вес, кг:
+6.5&lt;br&gt;
+Страна производства:
 Россия</t>
   </si>
 </sst>
@@ -706,7 +706,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -835,10 +835,10 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -861,10 +861,10 @@
         <v>19</v>
       </c>
       <c r="G6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -887,10 +887,10 @@
         <v>17</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -913,10 +913,10 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding cart and minor edits
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirilllahnov/Documents/Building_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCE054E-25C6-FF4B-8B8B-B3DD3A2768EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63A0743-7F85-5648-BC2C-D1C584E80243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-17420" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-16920" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Кровля" sheetId="1" r:id="rId1"/>
@@ -107,156 +107,20 @@
     <t>Хфрактеристики</t>
   </si>
   <si>
-    <t>Цвет
-Серый
-Тип продукта
-Металлический лист
-Внешний вид поверхности
-Гладкий
-Основной материал
-Сталь
-Длина (см)
-200
-Ширина (см)
-125
-Толщина (мм)
-0.35
-Размер (Д х Ш х В) (мм)
-2000х1250х0,35
-Вес, кг
-6.5
-Покрытие
-Оцинкованный
-Страна производства
-Россия</t>
-  </si>
-  <si>
     <t>Карнизная планка — это уголок, который устанавливается на обрешетку вплотную к свесу. Одно плечо этого уголка накрывает крайние бруски обрешетки или первые 100-150 мм сплошного настила, второе направлено вниз и образует вместе с водосточным желобом узел, который закрывает боковую грань обрешетки и торцы контрреек.</t>
   </si>
   <si>
-    <t>Тип продукта
-Планка карнизная
-Основной материал
-Полиэстер
-Толщина (мм)
-0.4
-Покрытие
-Без покрытия
-Цвет
-Коричневый
-Применение продукта
-Защищает нижнюю доску обрешётки и лобовую доску от воды
-Размер (Д х Ш х В) (мм)
-2000 х 200 х 0.4
-Вес, кг
-1.5
-Марка
-АРТСТРОЙСИТИ
-Страна производства
-Россия</t>
-  </si>
-  <si>
     <t>Снегозадержатель трубчатый длиной 3 м служит для предотвращения схода снега с кровли здания. Создает безопасные условия работы на крыше при ее ремонте или обслуживании, служит защитой водосточных систем. Снегозадержатель — незаменимый элемент кровли в регионах с обильными снегопадами. Крепится посредством кронштейнов саморезами с уплотнителями, совместим с разными кровельными покрытиями. Цвет конструкции — коричневый. Страна производства — Россия.</t>
-  </si>
-  <si>
-    <t>Тип продукта
-Снегозадержатель
-Основной материал
-Сталь
-Покрытие
-Оцинкованный
-Цветовая палитра по RAL
-RAL 8017
-Цвет
-Коричневый
-Размер (Д х Ш х В) (мм)
-3000х370х170
-Вес, кг
-4.6
-Страна производства
-Россия</t>
   </si>
   <si>
     <t xml:space="preserve">Профнастил С8 - это металлический лист с волнообразным профилем. Используется как облицовочный материал при строительстве заборов, гаражей, а так же обшивке стен и потолков.
 </t>
   </si>
   <si>
-    <t>Тип продукта
-Профнастил
-Основной материал
-Сталь
-Цветовая палитра
-Серый / серебристый
-Цветовая палитра по RAL
-Нет
-Площадь покрытия продуктом (м²)
-2.4
-Длина (см)
-200
-Ширина (см)
-120
-Толщина (мм)
-0.35
-Высота волны (мм)
-8
-Вес на м² (кг)
-3
-Вес, кг
-6.5
-Страна производства
-Россия</t>
-  </si>
-  <si>
     <t xml:space="preserve">Профнастил С20 — гофрированный лист серого цвета из оцинкованной холоднокатаной стали. Предназначен для заборов, обшивания стен и потолков изнутри, а также для кровли. Буква «С» в маркировке обозначает «стеновой», цифра указывает на высоту гофры в миллиметрах (большая волна).  </t>
   </si>
   <si>
-    <t>Тип продукта
-Профнастил
-Основной материал
-Сталь
-Цветовая палитра
-Зеленый
-Цветовая палитра по RAL
-RAL 6005
-Полезная площадь (м²)
-2.3
-Длина (см)
-200
-Ширина (см)
-120
-Толщина (мм)
-0.3
-Высота волны (мм)
-8
-Вес, кг
-5.99
-Страна производства
-Россия</t>
-  </si>
-  <si>
     <t>Профнастил С8 - это металлический лист с волнообразным профилем. Используется как облицовочный материал при строительстве заборов, гаражей, а так же обшивке стен и потолков.</t>
-  </si>
-  <si>
-    <t>Тип продукта
-Профнастил
-Основной материал
-Сталь
-Цветовая палитра
-Красный
-Цветовая палитра по RAL
-RAL 3005
-Длина (см)
-200
-Ширина (см)
-120
-Толщина (мм)
-0.3
-Высота волны (мм)
-8
-Вес, кг
-5.99
-Страна производства
-Россия</t>
   </si>
   <si>
     <t>Тип продукта:
@@ -283,6 +147,142 @@
 3,1&lt;br&gt;
 Вес, кг:
 6.5&lt;br&gt;
+Страна производства:
+Россия</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тип продукта:
+Профнастил&lt;br&gt;
+Основной материал:
+Сталь&lt;br&gt;
+Цветовая палитра:
+Зеленый&lt;br&gt;
+Цветовая палитра по RAL:
+RAL 6005&lt;br&gt;
+Полезная площадь (м²):
+2.3&lt;br&gt;
+Длина (см):
+200&lt;br&gt;
+Ширина (см):
+120&lt;br&gt;
+Толщина (мм):
+0.3&lt;br&gt;
+Высота волны (мм):
+8 &lt;br&gt;
+Вес, кг:
+5.99 &lt;br&gt;
+Страна производства:
+Россия </t>
+  </si>
+  <si>
+    <t>Тип продукта:
+Профнастил &lt;br&gt;
+Основной материал:
+Сталь&lt;br&gt;
+Цветовая палитра:
+Красный&lt;br&gt;
+Цветовая палитра по RAL:
+RAL 3005&lt;br&gt;
+Длина (см):
+200&lt;br&gt;
+Ширина (см):
+120&lt;br&gt;
+Толщина (мм):
+0.3&lt;br&gt;
+Высота волны (мм):
+8&lt;br&gt;
+Вес, кг:
+5.99&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>Тип продукта:
+Профнастил&lt;br&gt;
+Основной материал:
+Сталь&lt;br&gt;
+Цветовая палитра:
+Серый / серебристый&lt;br&gt;
+Цветовая палитра по RAL:
+Нет&lt;br&gt;
+Площадь покрытия продуктом (м²):
+2.4&lt;br&gt;
+Длина (см):
+200&lt;br&gt;
+Ширина (см):
+120&lt;br&gt;
+Толщина (мм):
+0.35&lt;br&gt;
+Высота волны (мм):
+8&lt;br&gt;
+Вес на м² (кг):
+3&lt;br&gt;
+Вес, кг:
+6.5&lt;br&gt;
+Страна производства:
+Россия</t>
+  </si>
+  <si>
+    <t>Тип продукта:
+Снегозадержатель &lt;br&gt;
+Основной материал:
+Сталь&lt;br&gt;
+Покрытие:
+Оцинкованный&lt;br&gt;
+Цветовая палитра по RAL:
+RAL 8017&lt;br&gt;
+Цвет:
+Коричневый&lt;br&gt;
+Размер (Д х Ш х В) (мм):
+3000х370х170&lt;br&gt;
+Вес, кг:
+4.6&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>Тип продукта:
+Планка карнизная&lt;br&gt;
+Основной материал:
+Полиэстер&lt;br&gt;
+Толщина (мм):
+0.4&lt;br&gt;
+Покрытие:
+Без покрытия&lt;br&gt;
+Цвет:
+Коричневый&lt;br&gt;
+Применение продукта:
+Защищает нижнюю доску обрешётки и лобовую доску от воды&lt;br&gt;
+Размер (Д х Ш х В) (мм):
+2000 х 200 х 0.4&lt;br&gt;
+Вес, кг:
+1.5&lt;br&gt;
+Марка:
+АРТСТРОЙСИТИ&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>Цвет:
+Серый&lt;br&gt;
+Тип продукта:
+Металлический лист&lt;br&gt;
+Внешний вид поверхности:
+Гладкий&lt;br&gt;
+Основной материал:
+Сталь&lt;br&gt;
+Длина (см):
+200&lt;br&gt;
+Ширина (см):
+125&lt;br&gt;
+Толщина (мм):
+0.35&lt;br&gt;
+Размер (Д х Ш х В) (мм):
+2000х1250х0,35&lt;br&gt;
+Вес, кг:
+6.5&lt;br&gt;
+Покрытие:
+Оцинкованный&lt;br&gt;
 Страна производства:
 Россия</t>
   </si>
@@ -372,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -390,9 +390,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -706,7 +703,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -739,10 +736,10 @@
       <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -762,11 +759,11 @@
       <c r="E2" s="5">
         <v>100</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>25</v>
+      <c r="H2" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -786,10 +783,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -809,10 +806,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -835,10 +832,10 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -860,11 +857,11 @@
       <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>31</v>
+      <c r="G6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -886,11 +883,11 @@
       <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>35</v>
+      <c r="G7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -913,10 +910,10 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scaled the generation of the product catalog
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirilllahnov/Documents/Building_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63A0743-7F85-5648-BC2C-D1C584E80243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB57D635-1659-F744-894A-08F2252A42A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-16920" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-16920" windowWidth="38400" windowHeight="19900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Кровля" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="3" r:id="rId2"/>
+    <sheet name="Сухие смеси и грунтовки" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
   <si>
     <t>ТИП</t>
   </si>
@@ -81,12 +81,6 @@
   </si>
   <si>
     <t>img/catalog/roof/4.jpeg</t>
-  </si>
-  <si>
-    <t>asaddd</t>
-  </si>
-  <si>
-    <t>ad</t>
   </si>
   <si>
     <t>Описание</t>
@@ -102,9 +96,6 @@
 Просто монтируется.
 Устойчив к воздействию ультрафиолета, атмосферных осадков и перепадам температур.
 Не теряет своих свойств в ходе эксплуатации.</t>
-  </si>
-  <si>
-    <t>Хфрактеристики</t>
   </si>
   <si>
     <t>Карнизная планка — это уголок, который устанавливается на обрешетку вплотную к свесу. Одно плечо этого уголка накрывает крайние бруски обрешетки или первые 100-150 мм сплошного настила, второе направлено вниз и образует вместе с водосточным желобом узел, который закрывает боковую грань обрешетки и торцы контрреек.</t>
@@ -286,12 +277,404 @@
 Страна производства:
 Россия</t>
   </si>
+  <si>
+    <t>Характеристики</t>
+  </si>
+  <si>
+    <t>Сухие смеси и грунтовки</t>
+  </si>
+  <si>
+    <t>Штукатурка</t>
+  </si>
+  <si>
+    <t>Штукатурка гипсовая Knauf Ротбанд 30 кг</t>
+  </si>
+  <si>
+    <t>Штукатурка гипсовая Knauf Ротбанд с полимерными добавками, обеспечивающими повышенную адгезию и легкость выполнения работы. Предназначена для выравнивания стен и потолков из бетона, кирпича, цементной штукатурки, поверхностей из пенополистирола, ЦСП. Рекомендуется для гладких бетонных потолочных и стеновых поверхностей.&lt;br&gt;
+Штукатурка подходит для отделки помещений с нормальной влажностью, а также в кухнях и ванных комнатах с покрытием, обеспечивающим защиту от увлажнения.
+Предназначена для внутренних работ.</t>
+  </si>
+  <si>
+    <t>Расход кг/м² при толщине слоя 10 мм:
+8.5&lt;br&gt;
+Максимальная толщина слоя (мм):
+50&lt;br&gt;
+Минимальная толщина слоя (мм):
+5&lt;br&gt;
+Жизнеспособность раствора (ч):
+0.5&lt;br&gt;
+Материал поверхности применения:
+Кирпич, Пазогребневая плита, Газобетонный блок&lt;br&gt;
+Место использования:
+Внутренний&lt;br&gt;
+Основной материал:
+Гипс&lt;br&gt;
+Применение продукта:
+Для внутренних работ&lt;br&gt;
+Расход воды на кг смеси, л:
+0.56&lt;br&gt;
+Адгезия (МПа):
+0,3&lt;br&gt;
+Прочность на сжатие (МПа):
+2.5&lt;br&gt;
+Размер фракции (мм):
+1.2&lt;br&gt;
+Цвет:
+Серый&lt;br&gt;
+Морозостойкость:
+Нет&lt;br&gt;
+Минимальная температура применения (°C):
+5&lt;br&gt;
+Максимальная температура применения (°C):
+30&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;
+Объем (кг):
+30&lt;br&gt;
+Марка:
+KNAUF</t>
+  </si>
+  <si>
+    <t>img/catalog/dry_mixes/1.jpeg</t>
+  </si>
+  <si>
+    <t>Штукатурка цементная Axton 25 кг</t>
+  </si>
+  <si>
+    <t>img/catalog/dry_mixes/2.jpeg</t>
+  </si>
+  <si>
+    <t>Цементная штукатурка Axton в упаковке на 25 кг – базовый материал для проведения отделочных работ. Используется для оштукатуривания фасадов, обеспечивая создание прочных монолитных поверхностей, готовых для чистовой отделки.&lt;br&gt;
+Цемент в качестве вяжущего гарантирует долговечность полученного материала.</t>
+  </si>
+  <si>
+    <t>Расход кг/м² при толщине слоя 10 мм:
+13.5&lt;br&gt;
+Максимальная толщина слоя (мм):
+20&lt;br&gt;
+Минимальная толщина слоя (мм):
+2&lt;br&gt;
+Жизнеспособность раствора (ч):
+3&lt;br&gt;
+Материал поверхности применения:
+Бетон, Газобетонный блок, Кирпич, Кирпич керамический, Силикат, Пазогребневая плита, Гипсокартон&lt;br&gt;
+Место использования:
+Внутренний / наружный&lt;br&gt;
+Основной материал:
+Цемент&lt;br&gt;
+Расход воды на кг смеси, л:
+0.22&lt;br&gt;
+Адгезия (МПа):
+0,5&lt;br&gt;
+Прочность на сжатие (МПа):
+7&lt;br&gt;
+Размер фракции (мм):
+0.63v
+Цвет:
+Серый&lt;br&gt;
+Класс морозостойкости:
+F50&lt;br&gt;
+Минимальная температура применения (°C):
+5&lt;br&gt;
+Максимальная температура применения (°C):
+30&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;
+Объем (кг):
+25&lt;br&gt;
+Марка:
+AXTON</t>
+  </si>
+  <si>
+    <t>Штукатурка гипсовая Волма Слой 30 кг</t>
+  </si>
+  <si>
+    <t>img/catalog/dry_mixes/3.jpeg</t>
+  </si>
+  <si>
+    <t>Штукатурка гипсовая Волма Слой 30 кг - сухая штукатурная смесь на основе натурального гипса, легкого заполнителя, минеральных наполнителей и модифицирующих добавок, обеспечивающих высокую адгезию, водоудерживающую способность и оптимальное время работы.&lt;br&gt;
+Применяется для выравнивания стен и потолков под оклейку обоями, покраску, облицовку керамической плиткой внутри помещений с нормальной относительной влажностью и температурой от +5°С до +30°С.
+Рекомендованный слой для стен 5-30 мм (максимально 60 мм), рекомендованный слой для выравнивания потолков 5-30 мм. При соблюдении технологии применения даёт глянцевую поверхность, не требующую дополнительного шпаклевания.&lt;br&gt;
+Для ручного нанесения.</t>
+  </si>
+  <si>
+    <t>Штукатурка цементная Axton 5 кг</t>
+  </si>
+  <si>
+    <t>Штукатурка цементная Axton — базовый материал для выравнивания стен и потолков при выраженных перепадах, для заделки дыр и трещин. Может использоваться внутри и снаружи зданий, во влажных помещениях. Содержание цемента в составе штукатурки обеспечивает прочность и долговечность покрытия.</t>
+  </si>
+  <si>
+    <t>Расход кг/м² при толщине слоя 10 мм:
+9&lt;br&gt;
+Максимальная толщина слоя (мм):
+60&lt;br&gt;
+Минимальная толщина слоя (мм):
+5&lt;br&gt;
+Жизнеспособность раствора (ч):
+0.75&lt;br&gt;
+Материал поверхности применения:
+Кирпич, Бетон, Пазогребневая плита, Гипсокартон&lt;br&gt;
+Место использования:
+Внутренний&lt;br&gt;
+Основной материал:
+Гипс&lt;br&gt;
+Применение продукта:
+Для внутренних работ&lt;br&gt;
+Расход воды на кг смеси, л:
+0.65&lt;br&gt;
+Адгезия (МПа):
+0,3&lt;br&gt;
+Прочность на сжатие (МПа):
+2&lt;br&gt;
+Размер фракции (мм):
+1.25&lt;br&gt;
+Цвет:
+Серый&lt;br&gt;
+Морозостойкость:
+Нет&lt;br&gt;
+Минимальная температура применения (°C):
+5&lt;br&gt;
+Максимальная температура применения (°C):
+30&lt;br&gt;
+Количество товара в паллете:
+45&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;
+Объем (кг):
+30&lt;br&gt;
+Марка:
+ВОЛМА</t>
+  </si>
+  <si>
+    <t>Расход кг/м² при толщине слоя 10 мм:
+13.5&lt;br&gt;
+Максимальная толщина слоя (мм):
+60&lt;br&gt;
+Минимальная толщина слоя (мм):
+5&lt;br&gt;
+Жизнеспособность раствора (ч):
+3&lt;br&gt;
+Материал поверхности применения:
+Бетон, Кирпич, Газобетонный блок, Кирпич керамический&lt;br&gt;
+Место использования:
+Внутренний / наружный&lt;br&gt;
+Основной материал:
+Цемент&lt;br&gt;
+Применение продукта:
+Для внутренних работ, Для наружных работ, Для работ во влажных помещениях&lt;br&gt;
+Расход воды на кг смеси, л:
+0.16v
+Адгезия (МПа):
+0,4&lt;br&gt;
+Прочность на сжатие (МПа):
+6&lt;br&gt;
+Размер фракции (мм):
+0.63&lt;br&gt;
+Время высыхания (ч):
+24&lt;br&gt;
+Цвет:
+Серый&lt;br&gt;
+Морозостойкость:
+Да&lt;br&gt;
+Класс морозостойкости:
+F50&lt;br&gt;
+Минимальная температура применения (°C):
+5&lt;br&gt;
+Максимальная температура применения (°C):
+30&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;
+Объем (кг):
+5&lt;br&gt;
+Марка:
+AXTON</t>
+  </si>
+  <si>
+    <t>Шпаклевки</t>
+  </si>
+  <si>
+    <t>img/catalog/dry_mixes/4.jpeg</t>
+  </si>
+  <si>
+    <t>Шпаклёвка полимерная суперфинишная Knauf Ротбанд Паста Профи 18 кг</t>
+  </si>
+  <si>
+    <t>«Ротбанд Паста Профи» - готовая пастообразная финишная шпаклевка на виниловой основе. Обладает повышенной белизной, адгезией и трещиностойкостью. Идеально подходит для тонкослойного (на сдир) шпаклевания поверхности. За счет высокой пластичности легко разравнивается и отлично заполняет мелкие неровности. После высыхания поверхность готова под финишное покрытие краской или обоями.&lt;br&gt;
+Применяется внутри помещений для финишного шпаклевания поверхности гипсокартонных или гипсоволокнистых листов, оштукатуренных и бетонных поверхностей, пазогребеневых плит, стеклохолста при подготовке под высококачественную окраску, оклейку обоями, перед нанесением венецианской штукатурки и других финишных материалов.</t>
+  </si>
+  <si>
+    <t>Минимальная толщина слоя (мм):
+0.2&lt;br&gt;
+Максимальная толщина слоя (мм):
+2&lt;br&gt;
+Место использования:
+Внутренний&lt;br&gt;
+Тип продукта (локальный):
+Суперфинишная шпатлевка&lt;br&gt;
+Вес нетто (кг):
+18&lt;br&gt;
+Тип применения:
+Универсальный&lt;br&gt;
+Состав:
+Акрил&lt;br&gt;
+Цвет:
+Белый&lt;br&gt;
+Минимальная температура применения (°C):
+10&lt;br&gt;
+Максимальная температура применения (°C):
+30&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;
+Марка:
+KNAUF</t>
+  </si>
+  <si>
+    <t>img/catalog/dry_mixes/5.jpeg</t>
+  </si>
+  <si>
+    <t>Шпаклёвка полимерная финишная Vetonit LR+ 5 кг</t>
+  </si>
+  <si>
+    <t>img/catalog/dry_mixes/6.jpeg</t>
+  </si>
+  <si>
+    <t>Финишная шпаклёвка Weber Vetonit LR+ (5 кг) – это смесь на основе тонкомолотого мрамора, предназначенная для финишного выравнивания потолков и стен перед покраской или поклейкой обоев. Подходит как для ручного нанесения, так и для распыления механическим способом.</t>
+  </si>
+  <si>
+    <t>Минимальная толщина слоя (мм):
+1&lt;br&gt;
+Максимальная толщина слоя (мм):
+5&lt;br&gt;
+Жизнеспособность раствора (ч):
+72&lt;br&gt;
+Место использования:
+Внутренний&lt;br&gt;
+Тип продукта (локальный):
+Финишная шпатлевка&lt;br&gt;
+Вес нетто (кг):
+5&lt;br&gt;
+Тип применения:
+Универсальный&lt;br&gt;
+Состав:
+Акрил&lt;br&gt;
+Цвет:
+Белый&lt;br&gt;
+Минимальная температура применения (°C):
+10&lt;br&gt;
+Максимальная температура применения (°C):
+30&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;
+Марка:
+VETONIT</t>
+  </si>
+  <si>
+    <t>Шпаклевка цементная влагостойкая Vetonit VH 20 кг</t>
+  </si>
+  <si>
+    <t>Шпаклевка финишная цементная влагостойкая Vetonit VH предназначена для выравнивания стен и потолков в помещениях с нормальным и повышенным уровнем влажности внутри и снаружи объектов. Наносится на основания перед финишным декоративным покрытием. Формирует матовый и гладкий защитный слой.&lt;br&gt;Безопасно для здоровья и природы. Этот товар имеет добровольный экологический сертификат, который гарантирует, что в составе изделия нет вредных для здоровья человека веществ.</t>
+  </si>
+  <si>
+    <t>Минимальная толщина слоя (мм):
+1&lt;br&gt;
+Максимальная толщина слоя (мм):
+4&lt;br&gt;
+Жизнеспособность раствора (ч):
+1.5&lt;br&gt;
+Место использования:
+Внутренний / наружный&lt;br&gt;
+Тип продукта (локальный):
+Базовая шпатлёвка&lt;br&gt;
+Вес нетто (кг):
+20&lt;br&gt;
+Тип применения:
+Универсальный&lt;br&gt;
+Состав:
+Цемент&lt;br&gt;
+Цвет:
+Белый&lt;br&gt;
+Минимальная температура применения (°C):
+10&lt;br&gt;
+Максимальная температура применения (°C):
+30&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;
+Марка:
+VETONIT</t>
+  </si>
+  <si>
+    <t>Грунтовка</t>
+  </si>
+  <si>
+    <t>Грунтовка глубокого проникновения Церезит CT17 10 л</t>
+  </si>
+  <si>
+    <t>img/catalog/dry_mixes/7.jpeg</t>
+  </si>
+  <si>
+    <t>img/catalog/dry_mixes/8.jpeg</t>
+  </si>
+  <si>
+    <t>Водно-дисперсионная грунтовка глубокого проникновения CT 17 предназначена для обработки поверхностей перед нанесением штукатурных и напольных смесей, плиточных клеев и т.д. Применяется для обработки всех видов впитывающих оснований: цементных штукатурок и стяжек, известковых и гипсовых штукатурок, легкого и ячеистого бетона, ангидритных стяжек, кладок из кирпича и природного камня, древесностружечных и древесноволокнистых плит, гипсокартона и т.д.&lt;br&gt;Обладает высокой проникающей способностью, снижает впитывающую способность оснований, связывает пыль, укрепляет поверхность, предотвращает пересыхание тонкослойных выравнивающих смесей, повышает адгезию материалов к основанию, повышает растекаемость напольных смесей и предотвращает появление пузырьков воздуха на выравнивающем слое.&lt;br&gt;Благодаря содержанию пигмента позволяет легко отличить обработанную поверхность.</t>
+  </si>
+  <si>
+    <t>Вес, кг:
+10.32&lt;br&gt;
+Тип продукта:
+Грунтовка глубокого проникновения&lt;br&gt;
+Расход (в л / м²):
+10&lt;br&gt;
+Площадь покрытия (м²):
+100&lt;br&gt;
+Время полного высыхания (ч):
+4&lt;br&gt;
+Минимальная температура применения (°C):
+5&lt;br&gt;
+Максимальная температура применения (°C):
+30&lt;br&gt;
+Запах:
+Без запаха&lt;br&gt;
+Материал поверхности применения:
+Цементно-известковая штукатурка, Бетонные подложки, Цемент, Бетон, Газобетонный блок, Гипсокартон&lt;br&gt;
+Цветовая палитра:
+Жёлтый / золотой&lt;br&gt;
+Срок годности (в месяцах):
+12&lt;br&gt;
+Готов к использованию:
+Да&lt;br&gt;
+Марка:
+ЦЕРЕЗИТ&lt;br&gt;
+Страна производства:
+Россия&lt;br&gt;
+Для влажных помещений:
+Да&lt;br&gt;
+Место использования:
+Внутренний / наружный&lt;br&gt;
+Количество слоев:
+1&lt;br&gt;
+Тип упаковки:
+Канистра&lt;br&gt;
+Время высыхания "на отлип" (в ч):
+1&lt;br&gt;
+Сухой остаток (%):
+0&lt;br&gt;
+Назначение:
+Для любых помещений&lt;br&gt;
+Предназначен для:
+Пол, Стена, Фасад&lt;br&gt;
+Состав:
+Акрил&lt;br&gt;
+Объем (л):
+10&lt;br&gt;
+Срок службы покрытия (лет):
+0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +688,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -314,7 +704,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -368,11 +758,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -395,6 +798,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -702,8 +1124,8 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -737,10 +1159,10 @@
         <v>15</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -760,10 +1182,10 @@
         <v>100</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -783,10 +1205,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -806,10 +1228,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -832,10 +1254,10 @@
         <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -858,10 +1280,10 @@
         <v>19</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -884,10 +1306,10 @@
         <v>17</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -910,10 +1332,10 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -923,22 +1345,255 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDEA5D6-51F9-124A-8930-2910D6524229}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="6" width="26.5" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" customWidth="1"/>
+    <col min="8" max="8" width="37.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>21</v>
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2">
+        <v>530</v>
+      </c>
+      <c r="E2">
+        <v>1232</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3">
+        <v>251</v>
+      </c>
+      <c r="E3">
+        <v>123</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4">
+        <v>506</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5">
+        <v>88</v>
+      </c>
+      <c r="E5">
+        <v>230</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>1585</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7">
+        <v>475</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8">
+        <v>702</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9">
+        <v>1253</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>